<commit_message>
2023-08-13 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/spritesheets/dunkbin_next_cosmetic.xlsx
+++ b/public/spritesheets/dunkbin_next_cosmetic.xlsx
@@ -32,12 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="[&gt;=10000]&quot;∞&quot;;[=1]0&quot; day&quot;;0&quot; days&quot;"/>
-    <numFmt numFmtId="165" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd&quot; &quot;hh&quot;:&quot;mm&quot;:&quot;ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>

</xml_diff>

<commit_message>
2023-08-17 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/spritesheets/dunkbin_next_cosmetic.xlsx
+++ b/public/spritesheets/dunkbin_next_cosmetic.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,7 +554,7 @@
         <v/>
       </c>
       <c r="G4">
-        <v>1081</v>
+        <v>822</v>
       </c>
       <c r="H4" t="str">
         <v/>
@@ -622,7 +622,7 @@
         <v/>
       </c>
     </row>
-    <row r="6">
+    <row r="6" xml:space="preserve">
       <c r="A6">
         <v>8</v>
       </c>
@@ -632,8 +632,9 @@
       <c r="C6" t="str">
         <v/>
       </c>
-      <c r="D6" t="str">
-        <v>Captain Panaka Star Wars</v>
+      <c r="D6" t="str" xml:space="preserve">
+        <v xml:space="preserve">Lelouch
+Code Geass</v>
       </c>
       <c r="E6" t="str">
         <v/>
@@ -686,7 +687,7 @@
         <v>Hat</v>
       </c>
       <c r="G7" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1117700050886336552/Panaka_Hat.png</v>
+        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933063843931/Dunk_Sweatling_Lelouch_HatHair_V2b_210x210.png</v>
       </c>
       <c r="H7" t="str">
         <v/>
@@ -774,7 +775,7 @@
         <v>Neck</v>
       </c>
       <c r="G9" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1117700050689212426/Panaka_Outfit.png</v>
+        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933399404614/Dunk_Sweatling_Lelouch_NeckClothes_V2b_210x210.png</v>
       </c>
       <c r="H9" t="str">
         <v/>
@@ -894,13 +895,13 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <v>lillava</v>
-      </c>
-      <c r="D12" t="str">
-        <v>(unknown)</v>
+        <v>omnipotent_0</v>
+      </c>
+      <c r="D12">
+        <v>42256416</v>
       </c>
       <c r="E12" t="str">
-        <v>65 days</v>
+        <v>257 days</v>
       </c>
       <c r="F12" t="str">
         <v/>
@@ -976,13 +977,13 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="str">
         <v/>
       </c>
       <c r="C14" t="str">
-        <v/>
+        <v>Omnipotent_0</v>
       </c>
       <c r="D14" t="str">
         <v/>
@@ -1009,62 +1010,106 @@
         <v/>
       </c>
       <c r="L14" t="str">
-        <v>shop item rows</v>
+        <v/>
       </c>
       <c r="M14" t="str">
-        <v>citb user(s)</v>
+        <v/>
       </c>
       <c r="N14" t="str">
-        <v>citb comment</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <v>shop item rows</v>
+      </c>
+      <c r="M15" t="str">
+        <v>citb user(s)</v>
+      </c>
+      <c r="N15" t="str">
+        <v>citb comment</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
         <v>21</v>
       </c>
-      <c r="B15" t="str">
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <v/>
-      </c>
-      <c r="D15" t="str">
-        <v/>
-      </c>
-      <c r="E15" t="str">
-        <v/>
-      </c>
-      <c r="F15" t="str">
-        <v/>
-      </c>
-      <c r="G15" t="str">
-        <v/>
-      </c>
-      <c r="H15" t="str">
-        <v/>
-      </c>
-      <c r="I15" t="str">
-        <v/>
-      </c>
-      <c r="J15" t="str">
-        <v/>
-      </c>
-      <c r="K15" t="str">
-        <v/>
-      </c>
-      <c r="L15">
-        <v>1081</v>
-      </c>
-      <c r="M15" t="str">
-        <v/>
-      </c>
-      <c r="N15" t="str">
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
+      <c r="E16" t="str">
+        <v/>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+      <c r="L16">
+        <v>822</v>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2023-08-19 update next cosmetic
</commit_message>
<xml_diff>
--- a/public/spritesheets/dunkbin_next_cosmetic.xlsx
+++ b/public/spritesheets/dunkbin_next_cosmetic.xlsx
@@ -589,7 +589,7 @@
         <v/>
       </c>
       <c r="H5">
-        <v>822</v>
+        <v>232</v>
       </c>
       <c r="I5" t="str">
         <v/>
@@ -662,8 +662,8 @@
         <v/>
       </c>
       <c r="E7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Lelouch
-Code Geass</v>
+        <v xml:space="preserve">Chaos Orb
+Path of Exile</v>
       </c>
       <c r="F7" t="str">
         <v/>
@@ -713,7 +713,7 @@
         <v>Hat</v>
       </c>
       <c r="H8" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933063843931/Dunk_Sweatling_Lelouch_HatHair_V2b_210x210.png</v>
+        <v>https://dunkbin.com/img/243.png</v>
       </c>
       <c r="I8" t="str">
         <v/>
@@ -795,7 +795,7 @@
         <v>Neck</v>
       </c>
       <c r="H10" t="str">
-        <v>https://cdn.discordapp.com/attachments/699111007649398865/1048523933399404614/Dunk_Sweatling_Lelouch_NeckClothes_V2b_210x210.png</v>
+        <v/>
       </c>
       <c r="I10" t="str">
         <v/>
@@ -906,13 +906,13 @@
         <v/>
       </c>
       <c r="D13" t="str">
-        <v>omnipotent_0</v>
+        <v>zakzak_channel</v>
       </c>
       <c r="E13">
-        <v>42256416</v>
+        <v>155860288</v>
       </c>
       <c r="F13" t="str">
-        <v>259 days</v>
+        <v>1009 days</v>
       </c>
       <c r="G13" t="str">
         <v/>
@@ -988,7 +988,7 @@
         <v/>
       </c>
       <c r="D15" t="str">
-        <v>Omnipotent_0</v>
+        <v>Galtz</v>
       </c>
       <c r="E15" t="str">
         <v/>

</xml_diff>